<commit_message>
work on ms projects
</commit_message>
<xml_diff>
--- a/Projektcontrolling/04_Kurzübung Projektcontrolling.xlsx
+++ b/Projektcontrolling/04_Kurzübung Projektcontrolling.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Source\repos\pmb\Projektcontrolling\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A260EF-762A-4395-9E78-92A130EC4D1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="15135"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28518" windowHeight="15138" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitspakete" sheetId="1" r:id="rId1"/>
@@ -220,7 +226,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -693,14 +699,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -738,9 +747,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -773,9 +782,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -808,9 +834,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -983,27 +1026,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83984375" customWidth="1"/>
+    <col min="7" max="7" width="13.578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.578125" customWidth="1"/>
+    <col min="9" max="10" width="18.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="13" t="s">
         <v>65</v>
       </c>
@@ -1035,7 +1078,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1061,7 +1104,7 @@
       </c>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -1087,7 +1130,7 @@
       <c r="I3" s="29"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -1117,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="17">
         <v>4</v>
       </c>
@@ -1147,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -1177,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -1207,7 +1250,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -1233,7 +1276,7 @@
       <c r="I8" s="29"/>
       <c r="J8" s="30"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -1263,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -1295,7 +1338,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="17">
         <v>10</v>
       </c>
@@ -1327,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -1357,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -1385,7 +1428,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -1413,7 +1456,7 @@
       <c r="I14" s="36"/>
       <c r="J14" s="38"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -1439,7 +1482,7 @@
       <c r="I15" s="42"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -1465,7 +1508,7 @@
       <c r="I16" s="29"/>
       <c r="J16" s="30"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="17">
         <v>16</v>
       </c>
@@ -1491,7 +1534,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -1517,7 +1560,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -1543,7 +1586,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="17">
         <v>19</v>
       </c>
@@ -1569,7 +1612,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -1597,7 +1640,7 @@
       <c r="I21" s="36"/>
       <c r="J21" s="38"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A22" s="11">
         <v>21</v>
       </c>

</xml_diff>